<commit_message>
Bug fixes and additional tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/devils_burdens/html_output/master.xlsx
+++ b/src/test/resources/devils_burdens/html_output/master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gnck/Documents/Code/race-timing/src/test/resources/devils_burdens/simple/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gnck/Documents/Code/race-timing/src/test/resources/devils_burdens/html_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45BF447-0B66-C844-AD51-2F0270008BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F77BA-B833-6349-B2B7-E8F76271AB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1430,11 +1430,11 @@
       </c>
       <c r="O6" s="1">
         <f>S6-MIN(O$10,R6)</f>
-        <v>5.0381944444444465E-2</v>
+        <v>-0.10924768518518518</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="2"/>
-        <v>0.15962962962962965</v>
+        <v>0</v>
       </c>
       <c r="R6" s="1">
         <f>B34</f>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="S6" s="1">
         <f>B35</f>
-        <v>0.15962962962962965</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1766,12 +1766,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0.15962962962962965</v>
-      </c>
+      <c r="B35" s="1"/>
       <c r="D35">
         <v>5</v>
       </c>

</xml_diff>